<commit_message>
Pointing system corrected for more accurate recommendations + code cleanup
</commit_message>
<xml_diff>
--- a/backend/app/Dogs.xlsx
+++ b/backend/app/Dogs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="174">
   <si>
     <t>Naam</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>Summary</t>
+  </si>
+  <si>
+    <t>Link</t>
   </si>
   <si>
     <t>Ara</t>
@@ -94,6 +97,9 @@
     <t>Ik vertrouw je niet meteen, maar ik ben gek op mensen die ik ken. We knuffelen samen, snoepen samen en spelen samen!</t>
   </si>
   <si>
+    <t>https://dierenasielgenk.be/honden/ara/</t>
+  </si>
+  <si>
     <t>Bailey</t>
   </si>
   <si>
@@ -125,6 +131,9 @@
     <t>Ik ben lief, zachtaardig en energiek. Ik zoek mensen die graag met mij willen trainen en knuffelen!</t>
   </si>
   <si>
+    <t>https://dierenasielgenk.be/honden/bailey-7/</t>
+  </si>
+  <si>
     <t>Bayka</t>
   </si>
   <si>
@@ -139,6 +148,9 @@
   </si>
   <si>
     <t>Ik ben een vriendelijke, blije en energieke hond. Als je actief met je hond bezig wil zijn, ben ik wellicht een leuke match!</t>
+  </si>
+  <si>
+    <t>https://dierenasielgenk.be/honden/bayka/</t>
   </si>
   <si>
     <t>Bessie</t>
@@ -153,10 +165,13 @@
 </t>
   </si>
   <si>
-    <t>https://dierenasielgenk.be/wp-content/uploads/2022/07/IMG_7240-1200x800.jpg</t>
+    <t>https://dierenasielgenk.be/wp-content/uploads/2022/07/IMG_7253-1200x800.jpg</t>
   </si>
   <si>
     <t>Ik volg heel graag mijn neus, maar mijn oren zijn wat moeilijker. Ik zoek een lief, beste maatje!</t>
+  </si>
+  <si>
+    <t>https://dierenasielgenk.be/honden/bessie/</t>
   </si>
   <si>
     <t>Bibi</t>
@@ -175,6 +190,9 @@
     <t>Wil jij Bibi een thuis bieden in een rustige omgeving? Dan krijg jij er een speels en liefdevol maatje voor het leven bij!</t>
   </si>
   <si>
+    <t>https://dierenasielgenk.be/honden/bibi-een-pientere-speelvogel/</t>
+  </si>
+  <si>
     <t>Biegel</t>
   </si>
   <si>
@@ -195,20 +213,7 @@
     <t>Ik ben een échte speurneus!</t>
   </si>
   <si>
-    <t>Bijoux</t>
-  </si>
-  <si>
-    <t>Na 11,5 jaar gewoond te hebben in een fijn thuis mocht Bijoux helaas niet mee naar het nieuwe thuis van de mensen en is ze afgestaan aan het asiel.
-Dit zachtaardige omaatje is graag bij de mensen en geniet ontzettend van aandacht. Ze moet in het asiel nog wel wennen en is niet graag alleen wat ze laat weten door wat te blaffen.
-Graag zal ze met haar nieuwe baasje knuffelen en op pad gaan. We zoeken een thuis voor haar met een leuk hondenvriendje (bij voorkeur een stabiele reu) die haar ook gezelschap kan geven. Ze kan bij kinderen vanaf 10 jaar en ze vereist een omheinde tuin. 
-Bijoux houdt erg van eten en kent de commando’s ‘zit’ en ‘poot’.
-Bijoux is op leeftijd, maar nog altijd fit en wil graag nog wat gezellige jaren doorbrengen bij lieve baasjes.</t>
-  </si>
-  <si>
-    <t>https://dierenasielgenk.be/wp-content/uploads/2022/10/EVIOCLICK_14-10-16-1200x800.jpg</t>
-  </si>
-  <si>
-    <t>Ik ben in de gouden jaren van mijn leven, maar ik ben nog altijd fit en wil graag nog wat gezellige jaren doorbrengen bij lieve baasjes!</t>
+    <t>https://dierenasielgenk.be/honden/biegel/</t>
   </si>
   <si>
     <t>Boelie</t>
@@ -230,6 +235,9 @@
     <t xml:space="preserve">Snuffelen, wandelen, apporteren, snoepen, zwemmen, trainen ... Ik ben een actieve hond die graag onderneemt! </t>
   </si>
   <si>
+    <t>https://dierenasielgenk.be/honden/boelie/</t>
+  </si>
+  <si>
     <t>Dario</t>
   </si>
   <si>
@@ -250,6 +258,9 @@
     <t>Ik ben wat onzeker, maar als je wat geduld hebt leer je me kennen als speelvogel en knuffelaar!</t>
   </si>
   <si>
+    <t>https://dierenasielgenk.be/honden/dario-2/</t>
+  </si>
+  <si>
     <t>Didi</t>
   </si>
   <si>
@@ -265,6 +276,9 @@
   </si>
   <si>
     <t>Ik ben wat bang en onzeker, maar als ik je vertrouw ben ik heel vriendelijk en wil ik graag knuffelen en spelen!</t>
+  </si>
+  <si>
+    <t>https://dierenasielgenk.be/honden/didi/</t>
   </si>
   <si>
     <t>Henkie</t>
@@ -288,6 +302,9 @@
     <t>Ik heb nog wat extra zorg en aandacht nodig, maar ik ben vrolijk, vriendelijk, speels en ik houd van aandacht!</t>
   </si>
   <si>
+    <t>https://dierenasielgenk.be/honden/henkie-3/</t>
+  </si>
+  <si>
     <t>Imara</t>
   </si>
   <si>
@@ -304,6 +321,9 @@
     <t>Ik heb nog wat zorg en leermomenten nodig, maar ik ben heel erg lief en zachtaardig!</t>
   </si>
   <si>
+    <t>https://dierenasielgenk.be/honden/imara/</t>
+  </si>
+  <si>
     <t>Junior</t>
   </si>
   <si>
@@ -318,6 +338,9 @@
   </si>
   <si>
     <t>Ik ben een vriendelijke hond die heel erg blij wordt van speurspellen, nieuwe commando's leren en wandelingen!</t>
+  </si>
+  <si>
+    <t>https://dierenasielgenk.be/honden/junior/</t>
   </si>
   <si>
     <t>Kita</t>
@@ -337,6 +360,9 @@
     <t xml:space="preserve">Ik ben actief, gek op eten en wil de wereld graag ontdekken met een leuk baasje. Mensen die graag hondensport willen beoefenen zijn ideaal! </t>
   </si>
   <si>
+    <t>https://dierenasielgenk.be/honden/kita-2/</t>
+  </si>
+  <si>
     <t>Lucky</t>
   </si>
   <si>
@@ -354,6 +380,9 @@
     <t>Ik ben onzeker maar wel erg nieuwsgierig en als ik je vertrouw ben ik een echte knuffelaar en speelvogel!</t>
   </si>
   <si>
+    <t>https://dierenasielgenk.be/honden/lucky-2/</t>
+  </si>
+  <si>
     <t>Max en Sky</t>
   </si>
   <si>
@@ -368,6 +397,9 @@
   </si>
   <si>
     <t>Double trouble, dubbel zoveel plezier en liefde!</t>
+  </si>
+  <si>
+    <t>https://dierenasielgenk.be/honden/max-en-sky-duoplaatsing/</t>
   </si>
   <si>
     <t>https://dierenasielgenk.be/wp-content/uploads/2022/09/ASIELGENK_WEB-25-1200x800.jpg</t>
@@ -397,6 +429,9 @@
     <t>Adopteer je mij, dan heb je een vriendin voor het leven! Mini muis voor maxi pret!</t>
   </si>
   <si>
+    <t>https://dierenasielgenk.be/honden/mini/</t>
+  </si>
+  <si>
     <t>Molly</t>
   </si>
   <si>
@@ -416,7 +451,13 @@
     <t>Zoek je een trouwe, leergierige metgezel om verder te laten kennismaken met het huiselijke leven? Dan is Molly misschien wel je ideale match!</t>
   </si>
   <si>
+    <t>https://dierenasielgenk.be/honden/molly/</t>
+  </si>
+  <si>
     <t>Poyraz</t>
+  </si>
+  <si>
+    <t>https://dierenasielgenk.be/honden/poyraz/</t>
   </si>
   <si>
     <t>Rita</t>
@@ -439,6 +480,9 @@
     <t>Ik ben geen allemansvriend, maar ik ben gek op snoepjes, spelen en knuffelen met bekende mensen!</t>
   </si>
   <si>
+    <t>https://dierenasielgenk.be/honden/rita/</t>
+  </si>
+  <si>
     <t>Rosa</t>
   </si>
   <si>
@@ -453,6 +497,9 @@
   </si>
   <si>
     <t>Ik zou heel graag een warme, fijne thuis vinden met geduldige mensen die me goed verzorgen en aandacht geven!</t>
+  </si>
+  <si>
+    <t>https://dierenasielgenk.be/honden/rosa-2/</t>
   </si>
   <si>
     <t>Ryna</t>
@@ -472,6 +519,9 @@
     <t>Ik moet nog wennen aan het leven binnen, maar ik ben erg nieuwsgierig en ik vind het heerlijk om te spelen en geaaid te worden!</t>
   </si>
   <si>
+    <t>https://dierenasielgenk.be/honden/ryna/</t>
+  </si>
+  <si>
     <t>Skippy</t>
   </si>
   <si>
@@ -486,6 +536,9 @@
   </si>
   <si>
     <t>Bied jij deze energieke herdershond een actief en liefdevol leven, dan wordt Skippy zeker en vast je beste vriendin!</t>
+  </si>
+  <si>
+    <t>https://dierenasielgenk.be/honden/skippy/</t>
   </si>
   <si>
     <t>Storm</t>
@@ -503,6 +556,9 @@
   </si>
   <si>
     <t>Ik ben een actieve Husky, ik weet heel goed wat ik wil!</t>
+  </si>
+  <si>
+    <t>https://dierenasielgenk.be/honden/storm/</t>
   </si>
   <si>
     <t>Thor</t>
@@ -523,6 +579,9 @@
     <t xml:space="preserve">Ik zou heel graag de rest van mijn leven doorbrengen op een plek waar ik graag gezien wordt, voldoende eten krijg en goed verzorgd wordt. </t>
   </si>
   <si>
+    <t>https://dierenasielgenk.be/honden/thor/</t>
+  </si>
+  <si>
     <t>Tipsie</t>
   </si>
   <si>
@@ -538,6 +597,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ik ben een hele zachte, lieve dame die ook wel houdt van wat mentale uitdagingen! Wordt jij mijn nieuwe maatje? </t>
+  </si>
+  <si>
+    <t>https://dierenasielgenk.be/honden/tipsie/</t>
   </si>
   <si>
     <t>Vicky</t>
@@ -561,6 +623,9 @@
     <t>Zoek je een energiek, aanhankelijk maatje dat je eerst vanop een veilig plekje kunt laten wennen aan het leven in huis? Dan is Vicky misschien wel de geknipte hond voor jou!</t>
   </si>
   <si>
+    <t>https://dierenasielgenk.be/honden/vicky/</t>
+  </si>
+  <si>
     <t>Zita</t>
   </si>
   <si>
@@ -579,6 +644,9 @@
     <t>Bent u op zoek naar een vrolijke en gezellige dame om leuke dingen mee te doen, maar ook om lekker mee in de zetel te liggen? Dan is Zita de juiste hond.</t>
   </si>
   <si>
+    <t>https://dierenasielgenk.be/honden/zita/</t>
+  </si>
+  <si>
     <t>Zora</t>
   </si>
   <si>
@@ -594,6 +662,9 @@
   </si>
   <si>
     <t>Ik speel graag, ik werk graag en ik ben leergierig, maar ook zeker aanhankelijkheid ontbreekt niet!</t>
+  </si>
+  <si>
+    <t>https://dierenasielgenk.be/honden/zora/</t>
   </si>
   <si>
     <t>Zuma</t>
@@ -615,6 +686,9 @@
   </si>
   <si>
     <t>Ik ben op zoek naar een baasje om mee te spelen en te speuren en om samen een mooie band op te bouwen!</t>
+  </si>
+  <si>
+    <t>https://dierenasielgenk.be/honden/zuma/</t>
   </si>
 </sst>
 </file>
@@ -952,6 +1026,7 @@
     <col customWidth="1" min="12" max="12" width="51.75"/>
     <col customWidth="1" min="13" max="13" width="32.75"/>
     <col customWidth="1" min="14" max="14" width="40.5"/>
+    <col customWidth="1" min="15" max="15" width="46.88"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
@@ -997,1341 +1072,1403 @@
       <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" ht="42.0" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="L2" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" ht="42.0" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="L3" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" ht="42.0" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="L4" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="5" ht="42.0" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="L5" s="5" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="6" ht="42.0" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="L6" s="5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>45</v>
+        <v>50</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="7" ht="42.0" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="J7" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>51</v>
+        <v>57</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="8" ht="42.0" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="L8" s="5" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>55</v>
+        <v>62</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="9" ht="42.0" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>21</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>19</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>59</v>
+        <v>68</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="10" ht="42.0" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="F10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="H10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="L10" s="5" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>64</v>
+        <v>73</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="11" ht="42.0" customHeight="1">
       <c r="A11" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="F11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="L11" s="5" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>68</v>
+        <v>79</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="12" ht="42.0" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="F12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="L12" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>72</v>
+        <v>82</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>73</v>
+        <v>84</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="13" ht="42.0" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>21</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="M13" s="7" t="s">
-        <v>76</v>
+        <v>87</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>77</v>
+        <v>89</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="14" ht="42.0" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="H14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="L14" s="5" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>81</v>
+        <v>94</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="15" ht="42.0" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>21</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>84</v>
+        <v>97</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>98</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>85</v>
+        <v>99</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="16" ht="42.0" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="L16" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="M16" s="7" t="s">
-        <v>88</v>
+        <v>102</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>89</v>
+        <v>104</v>
+      </c>
+      <c r="O16" s="6" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="17" ht="42.0" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="L17" s="5" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>93</v>
+        <v>104</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="18" ht="42.0" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="L18" s="5" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>93</v>
+        <v>110</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="19" ht="42.0" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="H19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="L19" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="O19" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" ht="42.0" customHeight="1">
+      <c r="A20" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="O20" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" ht="42.0" customHeight="1">
+      <c r="A21" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="I21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K19" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="M19" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="N19" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" ht="42.0" customHeight="1">
-      <c r="A20" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="M20" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="N20" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" ht="42.0" customHeight="1">
-      <c r="A21" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
+      <c r="J21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="N21" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="O21" s="6" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="22" ht="42.0" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="K22" s="4" t="s">
         <v>19</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="M22" s="6" t="s">
-        <v>106</v>
+        <v>125</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>126</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>107</v>
+        <v>127</v>
+      </c>
+      <c r="O22" s="6" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="23" ht="42.0" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="M23" s="7" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>111</v>
+        <v>132</v>
+      </c>
+      <c r="O23" s="6" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="24" ht="42.0" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K24" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I24" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="L24" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="M24" s="7" t="s">
-        <v>114</v>
+        <v>135</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>115</v>
+        <v>137</v>
+      </c>
+      <c r="O24" s="6" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="25" ht="42.0" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="H25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K25" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I25" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="L25" s="5" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>119</v>
+        <v>142</v>
+      </c>
+      <c r="O25" s="6" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="26" ht="42.0" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>21</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>123</v>
+        <v>147</v>
+      </c>
+      <c r="O26" s="6" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="27" ht="42.0" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K27" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="L27" s="5" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>127</v>
+        <v>152</v>
+      </c>
+      <c r="O27" s="6" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="28" ht="42.0" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="H28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="J28" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K28" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="L28" s="5" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="N28" s="5" t="s">
-        <v>131</v>
+        <v>157</v>
+      </c>
+      <c r="O28" s="6" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="29" ht="42.0" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>132</v>
+        <v>159</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>19</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>134</v>
+        <v>161</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>135</v>
+        <v>162</v>
+      </c>
+      <c r="O29" s="6" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="30" ht="42.0" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="H30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K30" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I30" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="L30" s="5" t="s">
-        <v>137</v>
+        <v>165</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="N30" s="5" t="s">
-        <v>139</v>
+        <v>167</v>
+      </c>
+      <c r="O30" s="6" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="31" ht="42.0" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>140</v>
+        <v>169</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>141</v>
+        <v>170</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
       <c r="N31" s="5" t="s">
-        <v>143</v>
+        <v>172</v>
+      </c>
+      <c r="O31" s="6" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="32" ht="42.0" customHeight="1">
-      <c r="A32" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L32" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="M32" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="N32" s="5" t="s">
-        <v>147</v>
-      </c>
+      <c r="A32" s="4"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
     </row>
     <row r="33" ht="42.0" customHeight="1">
       <c r="A33" s="4"/>
@@ -2474,7 +2611,6 @@
       <c r="H43" s="9"/>
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
     </row>
     <row r="44" ht="42.0" customHeight="1">
       <c r="A44" s="4"/>
@@ -2609,7 +2745,6 @@
       <c r="J54" s="9"/>
     </row>
     <row r="55" ht="42.0" customHeight="1">
-      <c r="A55" s="4"/>
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
@@ -2951,15 +3086,8 @@
       <c r="J85" s="9"/>
     </row>
     <row r="86" ht="42.0" customHeight="1">
-      <c r="B86" s="9"/>
-      <c r="C86" s="9"/>
-      <c r="D86" s="9"/>
-      <c r="E86" s="9"/>
-      <c r="F86" s="9"/>
-      <c r="G86" s="9"/>
-      <c r="H86" s="9"/>
-      <c r="I86" s="9"/>
-      <c r="J86" s="9"/>
+      <c r="D86" s="10"/>
+      <c r="G86" s="10"/>
     </row>
     <row r="87" ht="42.0" customHeight="1">
       <c r="D87" s="10"/>
@@ -6597,43 +6725,68 @@
       <c r="D995" s="10"/>
       <c r="G995" s="10"/>
     </row>
-    <row r="996" ht="42.0" customHeight="1">
-      <c r="D996" s="10"/>
-      <c r="G996" s="10"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="M2"/>
-    <hyperlink r:id="rId2" ref="M3"/>
-    <hyperlink r:id="rId3" ref="M4"/>
-    <hyperlink r:id="rId4" ref="M5"/>
-    <hyperlink r:id="rId5" ref="M6"/>
-    <hyperlink r:id="rId6" ref="M7"/>
-    <hyperlink r:id="rId7" ref="M8"/>
-    <hyperlink r:id="rId8" ref="M9"/>
-    <hyperlink r:id="rId9" ref="M10"/>
-    <hyperlink r:id="rId10" ref="M11"/>
-    <hyperlink r:id="rId11" ref="M12"/>
-    <hyperlink r:id="rId12" ref="M13"/>
-    <hyperlink r:id="rId13" ref="M14"/>
-    <hyperlink r:id="rId14" ref="M15"/>
-    <hyperlink r:id="rId15" ref="M16"/>
-    <hyperlink r:id="rId16" ref="M17"/>
-    <hyperlink r:id="rId17" ref="M18"/>
-    <hyperlink r:id="rId18" ref="M19"/>
-    <hyperlink r:id="rId19" ref="M20"/>
-    <hyperlink r:id="rId20" ref="M22"/>
-    <hyperlink r:id="rId21" ref="M23"/>
-    <hyperlink r:id="rId22" ref="M24"/>
-    <hyperlink r:id="rId23" ref="M25"/>
-    <hyperlink r:id="rId24" ref="M26"/>
-    <hyperlink r:id="rId25" ref="M27"/>
-    <hyperlink r:id="rId26" ref="M28"/>
-    <hyperlink r:id="rId27" ref="M29"/>
-    <hyperlink r:id="rId28" ref="M30"/>
-    <hyperlink r:id="rId29" ref="M31"/>
-    <hyperlink r:id="rId30" ref="M32"/>
+    <hyperlink r:id="rId2" ref="O2"/>
+    <hyperlink r:id="rId3" ref="M3"/>
+    <hyperlink r:id="rId4" ref="O3"/>
+    <hyperlink r:id="rId5" ref="M4"/>
+    <hyperlink r:id="rId6" ref="O4"/>
+    <hyperlink r:id="rId7" ref="M5"/>
+    <hyperlink r:id="rId8" ref="O5"/>
+    <hyperlink r:id="rId9" ref="M6"/>
+    <hyperlink r:id="rId10" ref="O6"/>
+    <hyperlink r:id="rId11" ref="M7"/>
+    <hyperlink r:id="rId12" ref="O7"/>
+    <hyperlink r:id="rId13" ref="M8"/>
+    <hyperlink r:id="rId14" ref="O8"/>
+    <hyperlink r:id="rId15" ref="M9"/>
+    <hyperlink r:id="rId16" ref="O9"/>
+    <hyperlink r:id="rId17" ref="M10"/>
+    <hyperlink r:id="rId18" ref="O10"/>
+    <hyperlink r:id="rId19" ref="M11"/>
+    <hyperlink r:id="rId20" ref="O11"/>
+    <hyperlink r:id="rId21" ref="M12"/>
+    <hyperlink r:id="rId22" ref="O12"/>
+    <hyperlink r:id="rId23" ref="M13"/>
+    <hyperlink r:id="rId24" ref="O13"/>
+    <hyperlink r:id="rId25" ref="M14"/>
+    <hyperlink r:id="rId26" ref="O14"/>
+    <hyperlink r:id="rId27" ref="M15"/>
+    <hyperlink r:id="rId28" ref="O15"/>
+    <hyperlink r:id="rId29" ref="M16"/>
+    <hyperlink r:id="rId30" ref="O16"/>
+    <hyperlink r:id="rId31" ref="M17"/>
+    <hyperlink r:id="rId32" ref="O17"/>
+    <hyperlink r:id="rId33" ref="M18"/>
+    <hyperlink r:id="rId34" ref="O18"/>
+    <hyperlink r:id="rId35" ref="M19"/>
+    <hyperlink r:id="rId36" ref="O19"/>
+    <hyperlink r:id="rId37" ref="O20"/>
+    <hyperlink r:id="rId38" ref="M21"/>
+    <hyperlink r:id="rId39" ref="O21"/>
+    <hyperlink r:id="rId40" ref="M22"/>
+    <hyperlink r:id="rId41" ref="O22"/>
+    <hyperlink r:id="rId42" ref="M23"/>
+    <hyperlink r:id="rId43" ref="O23"/>
+    <hyperlink r:id="rId44" ref="M24"/>
+    <hyperlink r:id="rId45" ref="O24"/>
+    <hyperlink r:id="rId46" ref="M25"/>
+    <hyperlink r:id="rId47" ref="O25"/>
+    <hyperlink r:id="rId48" ref="M26"/>
+    <hyperlink r:id="rId49" ref="O26"/>
+    <hyperlink r:id="rId50" ref="M27"/>
+    <hyperlink r:id="rId51" ref="O27"/>
+    <hyperlink r:id="rId52" ref="M28"/>
+    <hyperlink r:id="rId53" ref="O28"/>
+    <hyperlink r:id="rId54" ref="M29"/>
+    <hyperlink r:id="rId55" ref="O29"/>
+    <hyperlink r:id="rId56" ref="M30"/>
+    <hyperlink r:id="rId57" ref="O30"/>
+    <hyperlink r:id="rId58" ref="M31"/>
+    <hyperlink r:id="rId59" ref="O31"/>
   </hyperlinks>
-  <drawing r:id="rId31"/>
+  <drawing r:id="rId60"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated recommender system with filter. Added message function. Added Mongo DB functionality
</commit_message>
<xml_diff>
--- a/backend/app/Dogs.xlsx
+++ b/backend/app/Dogs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="158">
   <si>
     <t>Naam</t>
   </si>
@@ -281,30 +281,6 @@
     <t>https://dierenasielgenk.be/honden/didi/</t>
   </si>
   <si>
-    <t>Henkie</t>
-  </si>
-  <si>
-    <t>Eerder klein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deze leuke en lieve Lhasa Apso is na een hobbelig verleden op zoek naar een liefdevol thuis.
-Henkie is door een inbeslagname bij ons binnengebracht samen met nog enkele andere hondjes. Ze werden gebruikt voor de fok, maar kregen niet de juiste verzorging. Henkies vacht was vervilt, hij had kale plekken op zijn lijf en zijn ogen waren er slecht aan toe.
-Toch kwam gelijk zijn vrolijke en vriendelijke karakter naar boven ondanks dat hij in een nieuwe omgeving terecht kwam en zijn zicht vrijwel volledig ontbrak. Hij onderzocht zijn nieuwe plekje en was blij met de aandacht die hij kreeg. Hij is ook erg speels en vindt alle speeltjes leuk
-Op dit moment zit Henkie in een gastgezin waar hij veel liefde krijgt, hondenvriendjes heeft en ook de nodige medische zorg ontvangt. Ondertussen is hij gecastreerd, is zijn rechteroogje weggenomen en is zijn huid en vacht onder handen genomen. Om zijn andere oog te behouden wordt hij dagelijks intensief gezalfd en in de nabije toekomst heeft hij nog een operatie aan zijn knie nodig. We zoeken baasjes die deze zorg verder willen opvolgen.
-Henkie is 6 jaar, hij is zachtaardig, vriendelijk, onderzoekend en een levensgenieter. Hij wordt uitsluitend geplaatst bij een andere hond, hij kan ook bij kinderen vanaf 10 jaar en hij heeft nood aan een omheinde tuin. 
-In een nieuw thuis heeft Henkie veel baat bij een ander hondje en zullen aspecten zoals zindelijkheid en wandelen aan de riem verder opgebouwd moeten worden. In het gastgezin heeft hij hier al veel stappen in gemaakt.
-</t>
-  </si>
-  <si>
-    <t>https://dierenasielgenk.be/wp-content/uploads/2022/10/20221007_175756-1200x1814.jpg</t>
-  </si>
-  <si>
-    <t>Ik heb nog wat extra zorg en aandacht nodig, maar ik ben vrolijk, vriendelijk, speels en ik houd van aandacht!</t>
-  </si>
-  <si>
-    <t>https://dierenasielgenk.be/honden/henkie-3/</t>
-  </si>
-  <si>
     <t>Herman</t>
   </si>
   <si>
@@ -328,6 +304,9 @@
     <t>Imara</t>
   </si>
   <si>
+    <t>Eerder klein</t>
+  </si>
+  <si>
     <t xml:space="preserve">Imara werd samen met 14 andere Chihuahua’s en 8 katten in beslag genomen.
 Toen we onze eerste blik wierpen op Imara was het eigenlijk overduidelijk dat zij niet zomaar dik was, maar drachtig. Ze heeft hier in het asiel vier schattige pups ter wereld gebracht en deze liefdevol verzorgt, grootgebracht en uitgezwaaid. Nu is het aan deze lieve dame om ook haar eigen thuis te vinden.
 Ze is vriendelijk naar mensen en heel zachtaardig, maar kan mede door haar achtergrond met momenten onzeker zijn. Ook zal ze nog dingen moeten leren, zoals aan de riem wandelen.
@@ -342,25 +321,6 @@
   </si>
   <si>
     <t>https://dierenasielgenk.be/honden/imara/</t>
-  </si>
-  <si>
-    <t>Junior</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Junior werd samen met Tipsie en de pups in beslag genomen. De honden zaten in een vuil huis.
-Junior is een hele actieve hond, die een enorme focus heeft op tennisballen. Vermoedelijk is dit bij de vorige eigenaren gestimuleerd. We merken dat Junior graag met mensen activiteiten onderneemt, maar raden de tennisballen af. Speurspellen, nieuwe commando’s leren, wandelingen of zelfs joggen zijn activiteiten waar Junior heel blij van wordt.
-Junior is een vriendelijke hond, ook naar onbekende mensen. Hij kent de commando’s zit, af en poot en is duidelijk met hem gewerkt. Naast spelen is hij gek op eten en daar is een belangrijke regel bij Junior: wanneer hij iets lekkers heeft om te eten, wordt dit best geruild.
-Voor Junior is het belangrijk dat zijn nieuwe eigenaren het balspel niet stimuleren, maar hem wel voorzien in de behoefte om actief bezig te zijn. Een huis met een tuin is noodzakelijk. Hij wordt als enige hond geplaatst, eventueel bij volwassen kinderen.</t>
-  </si>
-  <si>
-    <t>https://dierenasielgenk.be/wp-content/uploads/2022/11/ASIELGENK_EVIOCLICK-34-1200x1800.jpg</t>
-  </si>
-  <si>
-    <t>Ik ben een vriendelijke hond die heel erg blij wordt van speurspellen, nieuwe commando's leren en wandelingen!</t>
-  </si>
-  <si>
-    <t>https://dierenasielgenk.be/honden/junior/</t>
   </si>
   <si>
     <t>Kita</t>
@@ -577,26 +537,6 @@
   </si>
   <si>
     <t>https://dierenasielgenk.be/honden/thor/</t>
-  </si>
-  <si>
-    <t>Tipsie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Tipsie werd samen met Junior en de pups in beslag genomen. De honden zaten in een vuil huis.
-We hebben Tipsie leren kennen als een hele zachte, lieve dame. Ze vindt het fijn om te knuffelen en speelt graag samen met de mens. Het is een actieve dame die activiteit graag wil afwisselen met fysiek contact. Ze is lichtjes onzeker, maar wanneer ze de tijd en ruimte krijgt om te gaan verkennen, wint haar nieuwsgierigheid van haar onzekerheid.
-Ze kent zit en poot en wanneer er lekkere beloningen te krijgen zijn, zal ze meer commando’s willen leren.
-Voor Tipsie is het belangrijk om zachtaardige mensen te vinden. Stemverheffingen zijn voor haar absoluut not-done.
-Tipsie kan bij een andere hond worden geplaatst; grotere kinderen zijn ook een optie. We zoeken voor haar mensen die graag wandelen/mentale uitdagingen willen bieden, maar ook zeker een hond zoeken om fijn mee te knuffelen.</t>
-  </si>
-  <si>
-    <t>https://dierenasielgenk.be/wp-content/uploads/2022/11/ASIELGENK_EVIOCLICK-28-1200x800.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ik ben een hele zachte, lieve dame die ook wel houdt van wat mentale uitdagingen! Wordt jij mijn nieuwe maatje? </t>
-  </si>
-  <si>
-    <t>https://dierenasielgenk.be/honden/tipsie/</t>
   </si>
   <si>
     <t>Vicky</t>
@@ -1323,7 +1263,7 @@
         <v>31</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>21</v>
@@ -1496,25 +1436,25 @@
         <v>53</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>22</v>
@@ -1523,42 +1463,42 @@
         <v>19</v>
       </c>
       <c r="L11" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="M11" s="6" t="s">
+      <c r="N11" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="O11" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="O11" s="6" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="12" ht="42.0" customHeight="1">
       <c r="A12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="D12" s="4" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>22</v>
@@ -1572,7 +1512,7 @@
       <c r="L12" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="M12" s="6" t="s">
+      <c r="M12" s="7" t="s">
         <v>83</v>
       </c>
       <c r="N12" s="5" t="s">
@@ -1590,19 +1530,19 @@
         <v>16</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>20</v>
@@ -1611,7 +1551,7 @@
         <v>22</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>19</v>
@@ -1619,7 +1559,7 @@
       <c r="L13" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="M13" s="7" t="s">
+      <c r="M13" s="6" t="s">
         <v>88</v>
       </c>
       <c r="N13" s="5" t="s">
@@ -1634,10 +1574,10 @@
         <v>91</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>54</v>
@@ -1658,7 +1598,7 @@
         <v>21</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>19</v>
@@ -1681,13 +1621,13 @@
         <v>96</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>19</v>
@@ -1696,42 +1636,42 @@
         <v>19</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="K15" s="4" t="s">
         <v>19</v>
       </c>
       <c r="L15" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="M15" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="M15" s="6" t="s">
-        <v>98</v>
-      </c>
       <c r="N15" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="O15" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" ht="42.0" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>54</v>
@@ -1758,30 +1698,30 @@
         <v>19</v>
       </c>
       <c r="L16" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="O16" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="M16" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="N16" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="O16" s="6" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="17" ht="42.0" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>19</v>
@@ -1790,31 +1730,31 @@
         <v>19</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>19</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="M17" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="O17" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="N17" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="O17" s="6" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="18" ht="42.0" customHeight="1">
@@ -1825,7 +1765,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>54</v>
@@ -1837,7 +1777,7 @@
         <v>19</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>20</v>
@@ -1846,10 +1786,10 @@
         <v>21</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L18" s="5" t="s">
         <v>109</v>
@@ -1872,28 +1812,28 @@
         <v>16</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>19</v>
@@ -1901,7 +1841,7 @@
       <c r="L19" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="M19" s="6" t="s">
+      <c r="M19" s="7" t="s">
         <v>115</v>
       </c>
       <c r="N19" s="5" t="s">
@@ -1922,33 +1862,33 @@
         <v>17</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L20" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="M20" s="6" t="s">
+      <c r="M20" s="7" t="s">
         <v>120</v>
       </c>
       <c r="N20" s="5" t="s">
@@ -1966,25 +1906,25 @@
         <v>16</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>18</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>22</v>
@@ -1995,7 +1935,7 @@
       <c r="L21" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="M21" s="7" t="s">
+      <c r="M21" s="6" t="s">
         <v>125</v>
       </c>
       <c r="N21" s="5" t="s">
@@ -2016,16 +1956,16 @@
         <v>17</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>20</v>
@@ -2034,7 +1974,7 @@
         <v>22</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="K22" s="4" t="s">
         <v>19</v>
@@ -2042,7 +1982,7 @@
       <c r="L22" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="M22" s="7" t="s">
+      <c r="M22" s="6" t="s">
         <v>130</v>
       </c>
       <c r="N22" s="5" t="s">
@@ -2057,7 +1997,7 @@
         <v>133</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>17</v>
@@ -2066,10 +2006,10 @@
         <v>18</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>31</v>
@@ -2078,7 +2018,7 @@
         <v>20</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>22</v>
@@ -2125,13 +2065,13 @@
         <v>20</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>32</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>139</v>
@@ -2151,19 +2091,19 @@
         <v>143</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>18</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>31</v>
@@ -2201,25 +2141,25 @@
         <v>16</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="F26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G26" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H26" s="4" t="s">
+      <c r="I26" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>32</v>
@@ -2245,19 +2185,19 @@
         <v>153</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>19</v>
@@ -2266,7 +2206,7 @@
         <v>20</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>32</v>
@@ -2288,145 +2228,43 @@
       </c>
     </row>
     <row r="28" ht="42.0" customHeight="1">
-      <c r="A28" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L28" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="M28" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="N28" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="O28" s="6" t="s">
-        <v>162</v>
-      </c>
+      <c r="A28" s="4"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
     </row>
     <row r="29" ht="42.0" customHeight="1">
-      <c r="A29" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L29" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="M29" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="N29" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="O29" s="6" t="s">
-        <v>167</v>
-      </c>
+      <c r="A29" s="4"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
     </row>
     <row r="30" ht="42.0" customHeight="1">
-      <c r="A30" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="M30" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="N30" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="O30" s="6" t="s">
-        <v>172</v>
-      </c>
+      <c r="A30" s="4"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
     </row>
     <row r="31" ht="42.0" customHeight="1">
       <c r="A31" s="4"/>
@@ -2530,7 +2368,6 @@
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
     </row>
     <row r="39" ht="42.0" customHeight="1">
       <c r="A39" s="4"/>
@@ -2543,7 +2380,6 @@
       <c r="H39" s="8"/>
       <c r="I39" s="8"/>
       <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
     </row>
     <row r="40" ht="42.0" customHeight="1">
       <c r="A40" s="4"/>
@@ -2556,7 +2392,6 @@
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
     </row>
     <row r="41" ht="42.0" customHeight="1">
       <c r="A41" s="4"/>
@@ -2667,7 +2502,6 @@
       <c r="J49" s="8"/>
     </row>
     <row r="50" ht="42.0" customHeight="1">
-      <c r="A50" s="4"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
@@ -2679,7 +2513,6 @@
       <c r="J50" s="8"/>
     </row>
     <row r="51" ht="42.0" customHeight="1">
-      <c r="A51" s="4"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
@@ -2691,7 +2524,6 @@
       <c r="J51" s="8"/>
     </row>
     <row r="52" ht="42.0" customHeight="1">
-      <c r="A52" s="4"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
@@ -3011,37 +2843,16 @@
       <c r="J80" s="8"/>
     </row>
     <row r="81" ht="42.0" customHeight="1">
-      <c r="B81" s="8"/>
-      <c r="C81" s="8"/>
-      <c r="D81" s="8"/>
-      <c r="E81" s="8"/>
-      <c r="F81" s="8"/>
-      <c r="G81" s="8"/>
-      <c r="H81" s="8"/>
-      <c r="I81" s="8"/>
-      <c r="J81" s="8"/>
+      <c r="D81" s="9"/>
+      <c r="G81" s="9"/>
     </row>
     <row r="82" ht="42.0" customHeight="1">
-      <c r="B82" s="8"/>
-      <c r="C82" s="8"/>
-      <c r="D82" s="8"/>
-      <c r="E82" s="8"/>
-      <c r="F82" s="8"/>
-      <c r="G82" s="8"/>
-      <c r="H82" s="8"/>
-      <c r="I82" s="8"/>
-      <c r="J82" s="8"/>
+      <c r="D82" s="9"/>
+      <c r="G82" s="9"/>
     </row>
     <row r="83" ht="42.0" customHeight="1">
-      <c r="B83" s="8"/>
-      <c r="C83" s="8"/>
-      <c r="D83" s="8"/>
-      <c r="E83" s="8"/>
-      <c r="F83" s="8"/>
-      <c r="G83" s="8"/>
-      <c r="H83" s="8"/>
-      <c r="I83" s="8"/>
-      <c r="J83" s="8"/>
+      <c r="D83" s="9"/>
+      <c r="G83" s="9"/>
     </row>
     <row r="84" ht="42.0" customHeight="1">
       <c r="D84" s="9"/>
@@ -6670,18 +6481,6 @@
     <row r="990" ht="42.0" customHeight="1">
       <c r="D990" s="9"/>
       <c r="G990" s="9"/>
-    </row>
-    <row r="991" ht="42.0" customHeight="1">
-      <c r="D991" s="9"/>
-      <c r="G991" s="9"/>
-    </row>
-    <row r="992" ht="42.0" customHeight="1">
-      <c r="D992" s="9"/>
-      <c r="G992" s="9"/>
-    </row>
-    <row r="993" ht="42.0" customHeight="1">
-      <c r="D993" s="9"/>
-      <c r="G993" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -6737,13 +6536,7 @@
     <hyperlink r:id="rId50" ref="O26"/>
     <hyperlink r:id="rId51" ref="M27"/>
     <hyperlink r:id="rId52" ref="O27"/>
-    <hyperlink r:id="rId53" ref="M28"/>
-    <hyperlink r:id="rId54" ref="O28"/>
-    <hyperlink r:id="rId55" ref="M29"/>
-    <hyperlink r:id="rId56" ref="O29"/>
-    <hyperlink r:id="rId57" ref="M30"/>
-    <hyperlink r:id="rId58" ref="O30"/>
   </hyperlinks>
-  <drawing r:id="rId59"/>
+  <drawing r:id="rId53"/>
 </worksheet>
 </file>
</xml_diff>